<commit_message>
updated the excel for multi run
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TCWPOMFILE.xlsx
+++ b/src/test/resources/excel/TCWPOMFILE.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\techbrain\eclipse-workspace\TCWPOM\src\test\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024B12FC-A310-42A1-83EE-DB3059B4B6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="addTaskTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +24,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Null Tasks</t>
+  </si>
+  <si>
+    <t>Automation skills</t>
+  </si>
+  <si>
+    <t>2nd task</t>
+  </si>
+  <si>
+    <t>null pointer</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +359,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Absence test case
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TCWPOMFILE.xlsx
+++ b/src/test/resources/excel/TCWPOMFILE.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\techbrain\eclipse-workspace\TCWPOM\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600C02CD-9259-452A-B345-4859D975045A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA1CE8C-6322-4739-BB13-D38B26F3A744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29055" yWindow="900" windowWidth="15060" windowHeight="14325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="addTaskTest" sheetId="1" r:id="rId1"/>
     <sheet name="addTimeSheetTest" sheetId="2" r:id="rId2"/>
+    <sheet name="addAbsenceTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>task</t>
   </si>
@@ -86,6 +87,51 @@
   </si>
   <si>
     <t>Adding the timesheet through Automation</t>
+  </si>
+  <si>
+    <t>Twentyone 21</t>
+  </si>
+  <si>
+    <t>absenceType</t>
+  </si>
+  <si>
+    <t>Fiscal Year</t>
+  </si>
+  <si>
+    <t>absenceStDt</t>
+  </si>
+  <si>
+    <t>20/08/2022</t>
+  </si>
+  <si>
+    <t>absenceEndDt</t>
+  </si>
+  <si>
+    <t>absenceStTime</t>
+  </si>
+  <si>
+    <t>absenceEndTime</t>
+  </si>
+  <si>
+    <t>05:30 PM</t>
+  </si>
+  <si>
+    <t>absenceLocation</t>
+  </si>
+  <si>
+    <t>Cramer Dentistry</t>
+  </si>
+  <si>
+    <t>absenceJob</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>absenceNotes</t>
+  </si>
+  <si>
+    <t>Adding the absence through automated test case</t>
   </si>
 </sst>
 </file>
@@ -93,8 +139,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-10409]hh:mm\ AM/PM;@"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-10409]hh:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -135,9 +181,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6C4EA1-1A02-47E2-A0CD-2A13DD69283F}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -522,4 +568,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8ABE68-3F9E-4A8B-9CCE-6EF36634D0D5}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Global settings test cases modified
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TCWPOMFILE.xlsx
+++ b/src/test/resources/excel/TCWPOMFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\techbrain\eclipse-workspace\TCWPOM\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30606816-7380-49B1-BB7E-0C28C220864C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E236A4DA-365B-4354-9459-932239757266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4395" yWindow="2085" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>task</t>
   </si>
@@ -176,12 +176,6 @@
   </si>
   <si>
     <t>Your Notes</t>
-  </si>
-  <si>
-    <t>2022-09-11</t>
-  </si>
-  <si>
-    <t>Manager Nine</t>
   </si>
   <si>
     <t>Hackshaw</t>
@@ -198,7 +192,7 @@
     <numFmt numFmtId="164" formatCode="[$-10409]hh:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,13 +205,6 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4C637B"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -240,14 +227,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,7 +699,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,10 +735,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>44</v>
@@ -787,7 +773,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,10 +809,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>44</v>

</xml_diff>